<commit_message>
Increase MaxInvest Storage Adapt Szenarios Existing Units
</commit_message>
<xml_diff>
--- a/data/Szenario_Default/Global_Parameters.xlsx
+++ b/data/Szenario_Default/Global_Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Szenario_Default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DB6F6F-8074-4E63-93D1-97B3F88FF2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674CAD56-45F5-4AD6-B945-1FFC98BF75A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1092,21 +1092,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1252,10 +1237,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1277,19 +1287,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change solver to Gurobi
</commit_message>
<xml_diff>
--- a/data/Szenario_Default/Global_Parameters.xlsx
+++ b/data/Szenario_Default/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Szenario_Default\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Server\Desktop\Michael\LEGO-Pyomo\data\Szenario_Default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674CAD56-45F5-4AD6-B945-1FFC98BF75A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DB3BFF-0D70-4CB0-9EBD-5DBD3F86E021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21075" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -59,6 +59,9 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -138,9 +141,6 @@
     <t>pSolver</t>
   </si>
   <si>
-    <t>highs</t>
-  </si>
-  <si>
     <t>Selected solver</t>
   </si>
   <si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>gurobi</t>
   </si>
 </sst>
 </file>
@@ -805,10 +808,10 @@
   <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
@@ -821,12 +824,12 @@
     <col min="9" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -846,7 +849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -858,32 +861,32 @@
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -894,12 +897,12 @@
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>9</v>
@@ -914,14 +917,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10"/>
       <c r="E10" s="10"/>
@@ -929,75 +932,75 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="9">
         <v>1E-3</v>
       </c>
       <c r="E12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="H12" s="13">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="G15" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="13">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="7" t="s">
         <v>5</v>
       </c>
@@ -1005,7 +1008,7 @@
       <c r="F17" s="12"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1016,7 +1019,7 @@
       <c r="F18" s="11"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1238,18 +1241,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1271,6 +1274,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1284,12 +1295,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Enable MIP gap for Gurobi and HiGHS solvers
Allows users to set the MIP gap for Gurobi and HiGHS solvers via the global parameters. The functionality is disabled when RMIP is enabled or when using different solvers.
</commit_message>
<xml_diff>
--- a/data/Szenario_Default/Global_Parameters.xlsx
+++ b/data/Szenario_Default/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Server\Desktop\Michael\LEGO-Pyomo\data\Szenario_Default\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\git\LEGO-Pyomo\data\Szenario_Default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DB3BFF-0D70-4CB0-9EBD-5DBD3F86E021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB5B84-779C-473B-9655-200493984165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21075" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -59,15 +59,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>[h]</t>
   </si>
@@ -187,6 +184,21 @@
   </si>
   <si>
     <t>Scaling factor for power values in input data (relative to 1MW)</t>
+  </si>
+  <si>
+    <t>Mip Gap</t>
+  </si>
+  <si>
+    <t>The MIP solver will terminate (with an optimal result) when the gap between the lower and upper objective bound is less than pMIPGap</t>
+  </si>
+  <si>
+    <t>pMIPGap</t>
+  </si>
+  <si>
+    <t>[%]</t>
+  </si>
+  <si>
+    <t>Relative MIP gap</t>
   </si>
   <si>
     <t>No</t>
@@ -408,16 +420,30 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -805,13 +831,13 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H19"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
@@ -824,12 +850,12 @@
     <col min="9" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -849,7 +875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -861,12 +887,12 @@
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>24</v>
@@ -881,12 +907,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -897,12 +923,12 @@
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>9</v>
@@ -917,81 +943,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="5" t="s">
+      <c r="C13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="13">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G14" s="11"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C15" s="9">
-        <v>9.9999999999999995E-7</v>
+        <v>1E-3</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>33</v>
@@ -1000,92 +1028,136 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="7" t="s">
+    <row r="16" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="9">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="13">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="5" t="s">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="3" t="s">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C22" s="9">
         <v>168</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H22" s="13">
         <v>168</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="26" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+  <conditionalFormatting sqref="C18">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="1" priority="19" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8:C9" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
       <formula1>"No, Yes"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C5 C12 C15" xr:uid="{13E44DF0-E318-4006-9E46-A03D51C3BE3C}"/>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{B1F27E54-4BFD-2D4B-9633-37AF83A83F57}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C5 C15 C18 C11" xr:uid="{13E44DF0-E318-4006-9E46-A03D51C3BE3C}"/>
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C22" xr:uid="{B1F27E54-4BFD-2D4B-9633-37AF83A83F57}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -1095,6 +1167,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1240,22 +1327,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1271,28 +1367,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>